<commit_message>
correction error res_bus & adding node_data as arg for some functions
</commit_message>
<xml_diff>
--- a/Sized_network_result_1.xlsx
+++ b/Sized_network_result_1.xlsx
@@ -3134,7 +3134,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.0335715005188572</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -3304,7 +3304,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>0.008800000000000001</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -3321,7 +3321,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>0.0176</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -3338,7 +3338,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="E14">
         <v>-0</v>
@@ -3355,7 +3355,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="E15">
         <v>-0</v>
@@ -3372,7 +3372,7 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -3474,7 +3474,7 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -3491,7 +3491,7 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="E23">
         <v>0</v>

</xml_diff>